<commit_message>
Search and Sort Implemented
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaurisha R Srivastav\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0EAB3B47-B074-43C8-8D48-434ADDA6441E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05069887-C067-40D3-96BC-94F93C15616E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B1CD5D8B-F437-4258-8F09-A92828887371}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B1CD5D8B-F437-4258-8F09-A92828887371}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="130">
   <si>
     <t>ITEM</t>
   </si>
@@ -102,9 +102,6 @@
     <t>turkey</t>
   </si>
   <si>
-    <t>whole wheat pasta</t>
-  </si>
-  <si>
     <t>soup</t>
   </si>
   <si>
@@ -192,15 +189,9 @@
     <t>chicken</t>
   </si>
   <si>
-    <t>pasta</t>
-  </si>
-  <si>
     <t>tomatoes</t>
   </si>
   <si>
-    <t>pancakes</t>
-  </si>
-  <si>
     <t>carrots</t>
   </si>
   <si>
@@ -388,6 +379,42 @@
   </si>
   <si>
     <t>napkins</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>meat</t>
+  </si>
+  <si>
+    <t>dry fruit</t>
+  </si>
+  <si>
+    <t>essentials</t>
+  </si>
+  <si>
+    <t>dairy</t>
+  </si>
+  <si>
+    <t>extras</t>
+  </si>
+  <si>
+    <t>fresh produce</t>
+  </si>
+  <si>
+    <t>beverage</t>
+  </si>
+  <si>
+    <t>ready to eat</t>
+  </si>
+  <si>
+    <t>whole wheat essentials</t>
+  </si>
+  <si>
+    <t>panready to eat</t>
   </si>
 </sst>
 </file>
@@ -748,972 +775,1817 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE9BF9AC-BA24-4A9E-AA5A-880653E116FF}">
-  <dimension ref="A1:B120"/>
+  <dimension ref="A1:E120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B120"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>205616461</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2">
+        <f t="shared" ref="C2:C65" ca="1" si="0">RANDBETWEEN(100,300)</f>
+        <v>194</v>
+      </c>
+      <c r="D2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>558925278</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <f t="shared" ca="1" si="0"/>
+        <v>134</v>
+      </c>
+      <c r="D3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>733001998</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <f t="shared" ca="1" si="0"/>
+        <v>260</v>
+      </c>
+      <c r="D4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <v>737104473</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <f t="shared" ca="1" si="0"/>
+        <v>184</v>
+      </c>
+      <c r="D5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <v>762451459</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <f t="shared" ca="1" si="0"/>
+        <v>196</v>
+      </c>
+      <c r="D6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
         <v>1304139212</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7">
+        <f t="shared" ca="1" si="0"/>
+        <v>282</v>
+      </c>
+      <c r="D7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
         <v>1304139220</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8">
+        <f t="shared" ca="1" si="0"/>
+        <v>121</v>
+      </c>
+      <c r="D8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
         <v>1304140894</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9">
+        <f t="shared" ca="1" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="D9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
         <v>1304146434</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10">
+        <f t="shared" ca="1" si="0"/>
+        <v>177</v>
+      </c>
+      <c r="D10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11">
         <v>1304146537</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C11">
+        <f t="shared" ca="1" si="0"/>
+        <v>133</v>
+      </c>
+      <c r="D11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12">
         <v>1304146744</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C12">
+        <f t="shared" ca="1" si="0"/>
+        <v>231</v>
+      </c>
+      <c r="D12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13">
         <v>1304168522</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C13">
+        <f t="shared" ca="1" si="0"/>
+        <v>230</v>
+      </c>
+      <c r="D13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14">
         <v>1304174778</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C14">
+        <f t="shared" ca="1" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="D14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15">
         <v>1304174867</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C15">
+        <f t="shared" ca="1" si="0"/>
+        <v>257</v>
+      </c>
+      <c r="D15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16">
         <v>1304174905</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <f t="shared" ca="1" si="0"/>
+        <v>242</v>
+      </c>
+      <c r="D16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17">
         <v>1304196046</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17">
+        <f t="shared" ca="1" si="0"/>
+        <v>118</v>
+      </c>
+      <c r="D17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18">
         <v>1304196062</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18">
+        <f t="shared" ca="1" si="0"/>
+        <v>190</v>
+      </c>
+      <c r="D18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19">
         <v>1304196070</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19">
+        <f t="shared" ca="1" si="0"/>
+        <v>127</v>
+      </c>
+      <c r="D19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20">
         <v>1304196135</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20">
+        <f t="shared" ca="1" si="0"/>
+        <v>198</v>
+      </c>
+      <c r="D20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21">
         <v>1304351475</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21">
+        <f t="shared" ca="1" si="0"/>
+        <v>235</v>
+      </c>
+      <c r="D21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22">
         <v>1304482596</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22">
+        <f t="shared" ca="1" si="0"/>
+        <v>157</v>
+      </c>
+      <c r="D22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23">
         <v>1304482634</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C23">
+        <f t="shared" ca="1" si="0"/>
+        <v>262</v>
+      </c>
+      <c r="D23" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24">
         <v>1304482685</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C24">
+        <f t="shared" ca="1" si="0"/>
+        <v>156</v>
+      </c>
+      <c r="D24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="B25">
         <v>1304488608</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C25">
+        <f t="shared" ca="1" si="0"/>
+        <v>221</v>
+      </c>
+      <c r="D25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>1304495396</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C26">
+        <f t="shared" ca="1" si="0"/>
+        <v>277</v>
+      </c>
+      <c r="D26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27">
         <v>1304511073</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27">
+        <f t="shared" ca="1" si="0"/>
+        <v>148</v>
+      </c>
+      <c r="D27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28">
         <v>1304511081</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C28">
+        <f t="shared" ca="1" si="0"/>
+        <v>256</v>
+      </c>
+      <c r="D28" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29">
         <v>1304511111</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C29">
+        <f t="shared" ca="1" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="D29" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30">
         <v>1304511124</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C30">
+        <f t="shared" ca="1" si="0"/>
+        <v>209</v>
+      </c>
+      <c r="D30" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31">
         <v>1304511138</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C31">
+        <f t="shared" ca="1" si="0"/>
+        <v>159</v>
+      </c>
+      <c r="D31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32">
         <v>1304511146</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C32">
+        <f t="shared" ca="1" si="0"/>
+        <v>167</v>
+      </c>
+      <c r="D32" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33">
         <v>1304511154</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C33">
+        <f t="shared" ca="1" si="0"/>
+        <v>234</v>
+      </c>
+      <c r="D33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34">
         <v>1304622193</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C34">
+        <f t="shared" ca="1" si="0"/>
+        <v>168</v>
+      </c>
+      <c r="D34" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35">
         <v>1304622223</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C35">
+        <f t="shared" ca="1" si="0"/>
+        <v>276</v>
+      </c>
+      <c r="D35" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36">
         <v>1304622428</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C36">
+        <f t="shared" ca="1" si="0"/>
+        <v>217</v>
+      </c>
+      <c r="D36" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37">
         <v>1304622452</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C37">
+        <f t="shared" ca="1" si="0"/>
+        <v>129</v>
+      </c>
+      <c r="D37" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38">
         <v>1304622460</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C38">
+        <f t="shared" ca="1" si="0"/>
+        <v>176</v>
+      </c>
+      <c r="D38" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39">
         <v>1304622622</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C39">
+        <f t="shared" ca="1" si="0"/>
+        <v>168</v>
+      </c>
+      <c r="D39" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40">
         <v>1304622657</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C40">
+        <f t="shared" ca="1" si="0"/>
+        <v>139</v>
+      </c>
+      <c r="D40" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41">
         <v>1304622665</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C41">
+        <f t="shared" ca="1" si="0"/>
+        <v>285</v>
+      </c>
+      <c r="D41" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42">
         <v>1304624498</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C42">
+        <f t="shared" ca="1" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="D42" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43">
         <v>1304624544</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C43">
+        <f t="shared" ca="1" si="0"/>
+        <v>118</v>
+      </c>
+      <c r="D43" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44">
         <v>1304651029</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C44">
+        <f t="shared" ca="1" si="0"/>
+        <v>139</v>
+      </c>
+      <c r="D44" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45">
         <v>1304651088</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C45">
+        <f t="shared" ca="1" si="0"/>
+        <v>214</v>
+      </c>
+      <c r="D45" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46">
         <v>1304651104</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C46">
+        <f t="shared" ca="1" si="0"/>
+        <v>274</v>
+      </c>
+      <c r="D46" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47">
         <v>1304651118</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C47">
+        <f t="shared" ca="1" si="0"/>
+        <v>223</v>
+      </c>
+      <c r="D47" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48">
         <v>1304651347</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C48">
+        <f t="shared" ca="1" si="0"/>
+        <v>151</v>
+      </c>
+      <c r="D48" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49">
         <v>1304665704</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C49">
+        <f t="shared" ca="1" si="0"/>
+        <v>234</v>
+      </c>
+      <c r="D49" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50">
         <v>1304665720</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C50">
+        <f t="shared" ca="1" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="D50" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51">
         <v>1304665784</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C51">
+        <f t="shared" ca="1" si="0"/>
+        <v>285</v>
+      </c>
+      <c r="D51" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52">
         <v>1403790965</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C52">
+        <f t="shared" ca="1" si="0"/>
+        <v>183</v>
+      </c>
+      <c r="D52" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53">
         <v>1412759676</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C53">
+        <f t="shared" ca="1" si="0"/>
+        <v>285</v>
+      </c>
+      <c r="D53" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54">
         <v>1451646526</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C54">
+        <f t="shared" ca="1" si="0"/>
+        <v>271</v>
+      </c>
+      <c r="D54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>122</v>
       </c>
       <c r="B55">
         <v>1457982633</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C55">
+        <f t="shared" ca="1" si="0"/>
+        <v>245</v>
+      </c>
+      <c r="D55" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B56">
         <v>1572671203</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C56">
+        <f t="shared" ca="1" si="0"/>
+        <v>126</v>
+      </c>
+      <c r="D56" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>129</v>
       </c>
       <c r="B57">
         <v>1879187396</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C57">
+        <f t="shared" ca="1" si="0"/>
+        <v>143</v>
+      </c>
+      <c r="D57" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B58">
         <v>1906987238</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C58">
+        <f t="shared" ca="1" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="D58" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B59">
         <v>1929099886</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C59">
+        <f t="shared" ca="1" si="0"/>
+        <v>291</v>
+      </c>
+      <c r="D59" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B60">
         <v>1987958179</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C60">
+        <f t="shared" ca="1" si="0"/>
+        <v>182</v>
+      </c>
+      <c r="D60" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B61">
         <v>3222000565</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C61">
+        <f t="shared" ca="1" si="0"/>
+        <v>121</v>
+      </c>
+      <c r="D61" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B62">
         <v>3227000754</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C62">
+        <f t="shared" ca="1" si="0"/>
+        <v>119</v>
+      </c>
+      <c r="D62" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B63">
         <v>3227001055</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C63">
+        <f t="shared" ca="1" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="D63" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B64">
         <v>3227001381</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C64">
+        <f t="shared" ca="1" si="0"/>
+        <v>103</v>
+      </c>
+      <c r="D64" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B65">
         <v>3292000971</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C65">
+        <f t="shared" ca="1" si="0"/>
+        <v>289</v>
+      </c>
+      <c r="D65" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B66">
         <v>3423470476</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C66">
+        <f t="shared" ref="C66:C120" ca="1" si="1">RANDBETWEEN(100,300)</f>
+        <v>215</v>
+      </c>
+      <c r="D66" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B67">
         <v>3602116004</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C67">
+        <f t="shared" ca="1" si="1"/>
+        <v>176</v>
+      </c>
+      <c r="D67" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B68">
         <v>4057362797</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C68">
+        <f t="shared" ca="1" si="1"/>
+        <v>237</v>
+      </c>
+      <c r="D68" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B69">
         <v>4057362843</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C69">
+        <f t="shared" ca="1" si="1"/>
+        <v>267</v>
+      </c>
+      <c r="D69" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B70">
         <v>4057362886</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C70">
+        <f t="shared" ca="1" si="1"/>
+        <v>263</v>
+      </c>
+      <c r="D70" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B71">
         <v>4057362894</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C71">
+        <f t="shared" ca="1" si="1"/>
+        <v>210</v>
+      </c>
+      <c r="D71" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B72">
         <v>4057362967</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C72">
+        <f t="shared" ca="1" si="1"/>
+        <v>256</v>
+      </c>
+      <c r="D72" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B73">
         <v>4057363823</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C73">
+        <f t="shared" ca="1" si="1"/>
+        <v>292</v>
+      </c>
+      <c r="D73" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B74">
         <v>4057368825</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C74">
+        <f t="shared" ca="1" si="1"/>
+        <v>224</v>
+      </c>
+      <c r="D74" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B75">
         <v>4057553908</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C75">
+        <f t="shared" ca="1" si="1"/>
+        <v>272</v>
+      </c>
+      <c r="D75" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B76">
         <v>5297000963</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C76">
+        <f t="shared" ca="1" si="1"/>
+        <v>216</v>
+      </c>
+      <c r="D76" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B77">
         <v>5357954771</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C77">
+        <f t="shared" ca="1" si="1"/>
+        <v>299</v>
+      </c>
+      <c r="D77" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B78">
         <v>5357955314</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C78">
+        <f t="shared" ca="1" si="1"/>
+        <v>202</v>
+      </c>
+      <c r="D78" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B79">
         <v>5357955454</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C79">
+        <f t="shared" ca="1" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="D79" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B80">
         <v>5357955743</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C80">
+        <f t="shared" ca="1" si="1"/>
+        <v>148</v>
+      </c>
+      <c r="D80" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B81">
         <v>5357955751</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C81">
+        <f t="shared" ca="1" si="1"/>
+        <v>131</v>
+      </c>
+      <c r="D81" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B82">
         <v>5357955786</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C82">
+        <f t="shared" ca="1" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="D82" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B83">
         <v>5357955832</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C83">
+        <f t="shared" ca="1" si="1"/>
+        <v>135</v>
+      </c>
+      <c r="D83" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B84">
         <v>5357955867</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C84">
+        <f t="shared" ca="1" si="1"/>
+        <v>262</v>
+      </c>
+      <c r="D84" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B85">
         <v>5357955905</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C85">
+        <f t="shared" ca="1" si="1"/>
+        <v>232</v>
+      </c>
+      <c r="D85" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B86">
         <v>5357955948</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C86">
+        <f t="shared" ca="1" si="1"/>
+        <v>297</v>
+      </c>
+      <c r="D86" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B87">
         <v>5357955972</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C87">
+        <f t="shared" ca="1" si="1"/>
+        <v>248</v>
+      </c>
+      <c r="D87" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B88">
         <v>5357956014</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C88">
+        <f t="shared" ca="1" si="1"/>
+        <v>220</v>
+      </c>
+      <c r="D88" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B89">
         <v>5357956111</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C89">
+        <f t="shared" ca="1" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="D89" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B90">
         <v>5357956227</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C90">
+        <f t="shared" ca="1" si="1"/>
+        <v>261</v>
+      </c>
+      <c r="D90" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B91">
         <v>6022600685</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C91">
+        <f t="shared" ca="1" si="1"/>
+        <v>272</v>
+      </c>
+      <c r="D91" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B92">
         <v>6022600744</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C92">
+        <f t="shared" ca="1" si="1"/>
+        <v>294</v>
+      </c>
+      <c r="D92" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B93">
         <v>6022600790</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C93">
+        <f t="shared" ca="1" si="1"/>
+        <v>191</v>
+      </c>
+      <c r="D93" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B94">
         <v>6022600804</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C94">
+        <f t="shared" ca="1" si="1"/>
+        <v>139</v>
+      </c>
+      <c r="D94" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B95">
         <v>6022600812</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C95">
+        <f t="shared" ca="1" si="1"/>
+        <v>214</v>
+      </c>
+      <c r="D95" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B96">
         <v>6040652705</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C96">
+        <f t="shared" ca="1" si="1"/>
+        <v>265</v>
+      </c>
+      <c r="D96" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B97">
         <v>6041134473</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C97">
+        <f t="shared" ca="1" si="1"/>
+        <v>229</v>
+      </c>
+      <c r="D97" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B98">
         <v>6041134494</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C98">
+        <f t="shared" ca="1" si="1"/>
+        <v>277</v>
+      </c>
+      <c r="D98" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B99">
         <v>6041134511</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C99">
+        <f t="shared" ca="1" si="1"/>
+        <v>259</v>
+      </c>
+      <c r="D99" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B100">
         <v>6053640972</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C100">
+        <f t="shared" ca="1" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="D100" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B101">
         <v>6117036094</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C101">
+        <f t="shared" ca="1" si="1"/>
+        <v>286</v>
+      </c>
+      <c r="D101" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B102">
         <v>6117043058</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C102">
+        <f t="shared" ca="1" si="1"/>
+        <v>162</v>
+      </c>
+      <c r="D102" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B103">
         <v>6152000416</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C103">
+        <f t="shared" ca="1" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="D103" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B104">
         <v>6162071103</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C104">
+        <f t="shared" ca="1" si="1"/>
+        <v>183</v>
+      </c>
+      <c r="D104" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B105">
         <v>6162751473</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C105">
+        <f t="shared" ca="1" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="D105" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B106">
         <v>6165151329</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C106">
+        <f t="shared" ca="1" si="1"/>
+        <v>117</v>
+      </c>
+      <c r="D106" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B107">
         <v>6165290582</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C107">
+        <f t="shared" ca="1" si="1"/>
+        <v>166</v>
+      </c>
+      <c r="D107" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B108">
         <v>6167061580</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C108">
+        <f t="shared" ca="1" si="1"/>
+        <v>294</v>
+      </c>
+      <c r="D108" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B109">
         <v>6169040335</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C109">
+        <f t="shared" ca="1" si="1"/>
+        <v>286</v>
+      </c>
+      <c r="D109" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B110">
         <v>6175005570</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C110">
+        <f t="shared" ca="1" si="1"/>
+        <v>218</v>
+      </c>
+      <c r="D110" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B111">
         <v>6175005589</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C111">
+        <f t="shared" ca="1" si="1"/>
+        <v>195</v>
+      </c>
+      <c r="D111" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B112">
         <v>7119018714</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C112">
+        <f t="shared" ca="1" si="1"/>
+        <v>251</v>
+      </c>
+      <c r="D112" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B113">
         <v>7535842801</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C113">
+        <f t="shared" ca="1" si="1"/>
+        <v>249</v>
+      </c>
+      <c r="D113" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B114">
         <v>7538650584</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C114">
+        <f t="shared" ca="1" si="1"/>
+        <v>157</v>
+      </c>
+      <c r="D114" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B115">
         <v>7539914718</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C115">
+        <f t="shared" ca="1" si="1"/>
+        <v>228</v>
+      </c>
+      <c r="D115" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B116">
         <v>7800558258</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C116">
+        <f t="shared" ca="1" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="D116" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B117">
         <v>7806397051</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C117">
+        <f t="shared" ca="1" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="D117" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B118">
         <v>7842953384</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C118">
+        <f t="shared" ca="1" si="1"/>
+        <v>271</v>
+      </c>
+      <c r="D118" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B119">
         <v>7883527428</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C119">
+        <f t="shared" ca="1" si="1"/>
+        <v>152</v>
+      </c>
+      <c r="D119" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B120">
         <v>7883633309</v>
+      </c>
+      <c r="C120">
+        <f t="shared" ca="1" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="D120" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>